<commit_message>
- fixed Nexial email notification so that email settings can be configured either System properties (i.e. `-D`),   `project.properties` or data sheets. - fixed wrong link in systemvars/index.md
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/org/nexial/core/model/TestScenarioTest1.data.xlsx
+++ b/src/test/resources/org/nexial/core/model/TestScenarioTest1.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10305"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10422"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/org/nexial/core/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B86C16F-927F-8843-8E1F-346BD07C572F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FFC7D5-748B-B64B-A72E-CF979CB73AC4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="12980" windowWidth="40960" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>1200</t>
   </si>
@@ -205,6 +205,9 @@
   <si>
     <t>nexial.verbose</t>
   </si>
+  <si>
+    <t>nobody@nowhere.com</t>
+  </si>
 </sst>
 </file>
 
@@ -222,15 +225,18 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -1071,7 +1077,7 @@
   <dimension ref="A1:AAA13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -4631,7 +4637,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>

</xml_diff>

<commit_message>
fixed failed unit tests
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/org/nexial/core/model/TestScenarioTest1.data.xlsx
+++ b/src/test/resources/org/nexial/core/model/TestScenarioTest1.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/org/nexial/core/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FFC7D5-748B-B64B-A72E-CF979CB73AC4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4369BD-F6DA-0E49-BDA7-4AFDD29FFD56}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12980" windowWidth="40960" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="12980" windowWidth="40960" windowHeight="12540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>1200</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>,</t>
-  </si>
-  <si>
-    <t>mliu@ep.com</t>
   </si>
   <si>
     <t>username</t>
@@ -429,7 +426,45 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1076,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1090,10 +1125,10 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -1798,7 +1833,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2507,7 +2542,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -3216,7 +3251,7 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -3925,7 +3960,7 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -4634,10 +4669,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -5343,7 +5378,7 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -6052,7 +6087,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -6761,10 +6796,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -7470,10 +7505,10 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -8179,7 +8214,7 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>1</v>
@@ -8888,10 +8923,10 @@
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -10300,23 +10335,23 @@
   </sheetData>
   <sheetProtection sheet="1" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A14:BBC1048576 C1:BBC13 A1:B12">
-    <cfRule type="containsBlanks" dxfId="28" priority="28">
+    <cfRule type="containsBlanks" dxfId="31" priority="28">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B1048576 B1:B12">
-    <cfRule type="expression" dxfId="27" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="6" stopIfTrue="1">
       <formula>OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1) = "sentry.scope"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="27" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A1048576 A1:A12">
-    <cfRule type="beginsWith" dxfId="25" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="28" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="24" priority="23" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="23" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10330,7 +10365,7 @@
   <dimension ref="A1:AAA21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -10343,7 +10378,7 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -11052,7 +11087,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -11761,10 +11796,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -12470,7 +12505,7 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -13179,10 +13214,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -13888,7 +13923,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -14597,14 +14632,14 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7"/>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>3</v>
@@ -15310,10 +15345,10 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -16018,7 +16053,7 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>1</v>
@@ -16726,16 +16761,16 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="E10"/>
       <c r="F10"/>
@@ -17439,10 +17474,10 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -18148,14 +18183,14 @@
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -18859,11 +18894,11 @@
     </row>
     <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13"/>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -19568,7 +19603,7 @@
     </row>
     <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>1</v>
@@ -20276,16 +20311,16 @@
     </row>
     <row r="15" spans="1:703">
       <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
@@ -20988,19 +21023,19 @@
     </row>
     <row r="16" spans="1:703">
       <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -21702,10 +21737,10 @@
     </row>
     <row r="17" spans="1:702">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17"/>
       <c r="D17" s="3" t="s">
@@ -22412,16 +22447,16 @@
     </row>
     <row r="18" spans="1:702">
       <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
@@ -23124,10 +23159,10 @@
     </row>
     <row r="19" spans="1:702">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -23832,10 +23867,10 @@
     </row>
     <row r="20" spans="1:702">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -24540,10 +24575,10 @@
     </row>
     <row r="21" spans="1:702">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -25249,51 +25284,64 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A22:BBC1048576 F1:BBC21">
-    <cfRule type="containsBlanks" dxfId="23" priority="12">
+    <cfRule type="containsBlanks" dxfId="26" priority="15">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:B1048576">
-    <cfRule type="expression" dxfId="22" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
       <formula>OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1) = "sentry.scope"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A1048576">
-    <cfRule type="beginsWith" dxfId="20" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="23" priority="10" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A22,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="22" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A22,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A22))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E12 A14:E21 A13 C13:E13">
-    <cfRule type="containsBlanks" dxfId="17" priority="6">
+  <conditionalFormatting sqref="A1:E4 A14:E21 A13 C13:E13 A6:E12 A5 C5:E5">
+    <cfRule type="containsBlanks" dxfId="20" priority="9">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B12 B14:B21 C13">
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B4 B14:B21 C13 B6:B12">
+    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
       <formula>OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1) = "sentry.scope"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="8" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A21">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="17" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="3" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="16" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(B5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1) = "sentry.scope"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25305,7 +25353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AAA5"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -25319,14 +25367,14 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1"/>
       <c r="D1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -26030,10 +26078,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -26739,11 +26787,11 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3"/>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -27448,13 +27496,13 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4"/>
       <c r="E4"/>
@@ -28159,14 +28207,14 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5"/>
       <c r="D5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
@@ -28870,50 +28918,50 @@
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A6:BBC1048576 E1:BBC5">
-    <cfRule type="containsBlanks" dxfId="11" priority="12">
+    <cfRule type="containsBlanks" dxfId="14" priority="12">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B1048576">
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="8" stopIfTrue="1">
       <formula>OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1) = "sentry.scope"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A1048576">
-    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="11" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="10" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="6" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D5">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B5">
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1) = "sentry.scope"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 7) = "sentry."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A5">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="4" priority="3" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>